<commit_message>
Updated stats for 650t min viable catch
</commit_message>
<xml_diff>
--- a/mserproject/statistics/WCVI_HerringObjectiveTable.xlsx
+++ b/mserproject/statistics/WCVI_HerringObjectiveTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13700" yWindow="440" windowWidth="19860" windowHeight="20480" tabRatio="500"/>
+    <workbookView xWindow="18560" yWindow="740" windowWidth="27960" windowHeight="23260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="WCVI_HerringObjectiveTable" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="42">
   <si>
     <t>Scenario</t>
   </si>
@@ -144,13 +144,22 @@
   </si>
   <si>
     <t>P(Bt &gt; Bave-prod)</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>P(Ct &lt; 650t)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -184,23 +193,30 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Cambria"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -255,19 +271,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom style="medium">
         <color auto="1"/>
@@ -331,132 +334,149 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -733,117 +753,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L40"/>
+  <dimension ref="B1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:L40"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="6"/>
+    <col min="1" max="1" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="3" t="s">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="3" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="4" t="s">
         <v>19</v>
       </c>
       <c r="J1" s="5"/>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="6"/>
+      <c r="L1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="5"/>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1"/>
+      <c r="M1" s="6"/>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="10" t="s">
+      <c r="I2" s="10"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="M2" s="13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="13" t="s">
+    <row r="3" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="16" t="s">
         <v>29</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="M3" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+    <row r="4" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="16" t="s">
         <v>34</v>
       </c>
       <c r="G4" s="15" t="s">
@@ -855,1231 +881,1342 @@
       <c r="I4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="J4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="M4" s="16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="6" t="s">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="20">
         <v>10</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="21">
         <v>0.88400000000000001</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="22">
         <v>0.60933333333333295</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="21">
         <v>0.45733333333333298</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="22">
         <v>0.42399999999999999</v>
       </c>
-      <c r="I5" s="22">
-        <v>6.8145387673812996</v>
-      </c>
-      <c r="J5" s="23">
+      <c r="I5" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="24">
         <v>0.13411958684552999</v>
       </c>
-      <c r="K5" s="24">
+      <c r="K5" s="22">
+        <v>1</v>
+      </c>
+      <c r="L5" s="25">
         <v>0.61266666666666703</v>
       </c>
-      <c r="L5" s="25">
+      <c r="M5" s="26">
         <v>0.39800000000000002</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="6" t="s">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="20">
         <v>6</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="27">
         <v>0.87</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="26">
         <v>0.54933333333333301</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="27">
         <v>0.39333333333333298</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="26">
         <v>0.377</v>
       </c>
-      <c r="I6" s="27">
+      <c r="I6" s="28">
         <v>16.4879877909074</v>
       </c>
-      <c r="J6" s="28">
+      <c r="J6" s="29">
         <v>1.71558949282353</v>
       </c>
-      <c r="K6" s="24">
+      <c r="K6" s="26">
+        <v>0.25133333333333302</v>
+      </c>
+      <c r="L6" s="25">
         <v>0.55066666666666697</v>
       </c>
-      <c r="L6" s="25">
+      <c r="M6" s="26">
         <v>0.34133333333333299</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="6" t="s">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B7" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="20">
         <v>9</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="27">
         <v>0.86133333333333295</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="26">
         <v>0.54266666666666696</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="27">
         <v>0.38800000000000001</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="26">
         <v>0.371</v>
       </c>
-      <c r="I7" s="27">
+      <c r="I7" s="28">
         <v>13.139599702317501</v>
       </c>
-      <c r="J7" s="28">
+      <c r="J7" s="29">
         <v>1.8555063997582699</v>
       </c>
-      <c r="K7" s="24">
+      <c r="K7" s="26">
+        <v>0.140666666666667</v>
+      </c>
+      <c r="L7" s="25">
         <v>0.54400000000000004</v>
       </c>
-      <c r="L7" s="25">
+      <c r="M7" s="26">
         <v>0.336666666666667</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="6" t="s">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B8" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="20">
         <v>3</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="27">
         <v>0.86133333333333295</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="26">
         <v>0.539333333333333</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="27">
         <v>0.38400000000000001</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="26">
         <v>0.36799999999999999</v>
       </c>
-      <c r="I8" s="27">
+      <c r="I8" s="28">
         <v>8.2551365679722899</v>
       </c>
-      <c r="J8" s="28">
+      <c r="J8" s="29">
         <v>1.84934234251611</v>
       </c>
-      <c r="K8" s="24">
+      <c r="K8" s="26">
+        <v>0.169333333333333</v>
+      </c>
+      <c r="L8" s="25">
         <v>0.54200000000000004</v>
       </c>
-      <c r="L8" s="25">
+      <c r="M8" s="26">
         <v>0.33533333333333298</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B9" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="20">
         <v>5</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="27">
         <v>0.85733333333333295</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="26">
         <v>0.47</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="27">
         <v>0.316</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="26">
         <v>0.316</v>
       </c>
-      <c r="I9" s="27">
+      <c r="I9" s="28">
         <v>39.071455858871097</v>
       </c>
-      <c r="J9" s="28">
+      <c r="J9" s="29">
         <v>3.6332789651735098</v>
       </c>
-      <c r="K9" s="24">
+      <c r="K9" s="26">
+        <v>0.26733333333333298</v>
+      </c>
+      <c r="L9" s="25">
         <v>0.46933333333333299</v>
       </c>
-      <c r="L9" s="25">
+      <c r="M9" s="26">
         <v>0.26933333333333298</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="6" t="s">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B10" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="20">
         <v>8</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="27">
         <v>0.84466666666666701</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="26">
         <v>0.46200000000000002</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="27">
         <v>0.31333333333333302</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="26">
         <v>0.31</v>
       </c>
-      <c r="I10" s="27">
+      <c r="I10" s="28">
         <v>36.329493301892597</v>
       </c>
-      <c r="J10" s="28">
+      <c r="J10" s="29">
         <v>3.7800071688649899</v>
       </c>
-      <c r="K10" s="24">
+      <c r="K10" s="26">
+        <v>0.14333333333333301</v>
+      </c>
+      <c r="L10" s="25">
         <v>0.46</v>
       </c>
-      <c r="L10" s="25">
+      <c r="M10" s="26">
         <v>0.26466666666666699</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="6" t="s">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B11" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="20">
         <v>2</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="27">
         <v>0.84399999999999997</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="26">
         <v>0.460666666666667</v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="27">
         <v>0.31266666666666698</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="26">
         <v>0.308</v>
       </c>
-      <c r="I11" s="27">
+      <c r="I11" s="28">
         <v>34.319906815785203</v>
       </c>
-      <c r="J11" s="28">
+      <c r="J11" s="29">
         <v>3.7929911685920401</v>
       </c>
-      <c r="K11" s="24">
+      <c r="K11" s="26">
+        <v>0.17733333333333301</v>
+      </c>
+      <c r="L11" s="25">
         <v>0.460666666666667</v>
       </c>
-      <c r="L11" s="25">
+      <c r="M11" s="26">
         <v>0.26533333333333298</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="6" t="s">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B12" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="20">
         <v>4</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="27">
         <v>0.77933333333333299</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="26">
         <v>0.32933333333333298</v>
       </c>
-      <c r="G12" s="26">
+      <c r="G12" s="27">
         <v>0.19600000000000001</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="26">
         <v>0.22</v>
       </c>
-      <c r="I12" s="27">
+      <c r="I12" s="28">
         <v>47.416619630679399</v>
       </c>
-      <c r="J12" s="28">
+      <c r="J12" s="29">
         <v>6.23045086152925</v>
       </c>
-      <c r="K12" s="24">
+      <c r="K12" s="26">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="L12" s="25">
         <v>0.32400000000000001</v>
       </c>
-      <c r="L12" s="25">
+      <c r="M12" s="26">
         <v>0.161333333333333</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="6" t="s">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B13" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="20">
         <v>1</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="27">
         <v>0.754</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="26">
         <v>0.30333333333333301</v>
       </c>
-      <c r="G13" s="26">
+      <c r="G13" s="27">
         <v>0.18666666666666701</v>
       </c>
-      <c r="H13" s="25">
+      <c r="H13" s="26">
         <v>0.20799999999999999</v>
       </c>
-      <c r="I13" s="27">
+      <c r="I13" s="28">
         <v>41.277353832446998</v>
       </c>
-      <c r="J13" s="28">
+      <c r="J13" s="29">
         <v>6.6588888275351303</v>
       </c>
-      <c r="K13" s="24">
+      <c r="K13" s="26">
+        <v>0.206666666666667</v>
+      </c>
+      <c r="L13" s="25">
         <v>0.30333333333333301</v>
       </c>
-      <c r="L13" s="25">
+      <c r="M13" s="26">
         <v>0.15</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B14" s="6" t="s">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B14" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="20">
         <v>7</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="26">
+      <c r="E14" s="27">
         <v>0.74333333333333296</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="26">
         <v>0.30333333333333301</v>
       </c>
-      <c r="G14" s="26">
+      <c r="G14" s="27">
         <v>0.18533333333333299</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14" s="26">
         <v>0.20899999999999999</v>
       </c>
-      <c r="I14" s="27">
+      <c r="I14" s="28">
         <v>40.311754715793498</v>
       </c>
-      <c r="J14" s="28">
+      <c r="J14" s="29">
         <v>6.5569879136786398</v>
       </c>
-      <c r="K14" s="24">
+      <c r="K14" s="26">
+        <v>0.135333333333333</v>
+      </c>
+      <c r="L14" s="25">
         <v>0.30333333333333301</v>
       </c>
-      <c r="L14" s="25">
+      <c r="M14" s="26">
         <v>0.148666666666667</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C15" s="19"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="24"/>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="30"/>
       <c r="L15" s="25"/>
-    </row>
-    <row r="16" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="13" t="s">
+      <c r="M15" s="26"/>
+    </row>
+    <row r="16" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="16" t="s">
+      <c r="I16" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="J16" s="15" t="s">
+      <c r="J16" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="K16" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="L16" s="15" t="s">
+      <c r="M16" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
+    <row r="17" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="15" t="s">
         <v>35</v>
       </c>
       <c r="H17" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="I17" s="16" t="s">
+      <c r="I17" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="J17" s="15" t="s">
+      <c r="J17" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="K17" s="15" t="s">
+      <c r="K17" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="L17" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="L17" s="15" t="s">
+      <c r="M17" s="16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="6" t="s">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B18" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="30">
+      <c r="C18" s="32">
         <v>10</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="27">
         <v>0.77800000000000002</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="26">
         <v>0.394666666666667</v>
       </c>
-      <c r="G18" s="26">
+      <c r="G18" s="27">
         <v>0.26600000000000001</v>
       </c>
-      <c r="H18" s="25">
+      <c r="H18" s="26">
         <v>0.31900000000000001</v>
       </c>
-      <c r="I18" s="27">
-        <v>10.785918112867099</v>
-      </c>
-      <c r="J18" s="28">
+      <c r="I18" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="J18" s="29">
         <v>0.12765536253504001</v>
       </c>
-      <c r="K18" s="24">
+      <c r="K18" s="26">
+        <v>1</v>
+      </c>
+      <c r="L18" s="25">
         <v>0.39533333333333298</v>
       </c>
-      <c r="L18" s="25">
+      <c r="M18" s="26">
         <v>0.22600000000000001</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="6" t="s">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B19" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="30">
+      <c r="C19" s="32">
         <v>6</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="27">
         <v>0.74133333333333296</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="26">
         <v>0.34666666666666701</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G19" s="27">
         <v>0.227333333333333</v>
       </c>
-      <c r="H19" s="25">
+      <c r="H19" s="26">
         <v>0.28399999999999997</v>
       </c>
-      <c r="I19" s="27">
+      <c r="I19" s="28">
         <v>29.434403925325999</v>
       </c>
-      <c r="J19" s="28">
+      <c r="J19" s="29">
         <v>1.51803963328765</v>
       </c>
-      <c r="K19" s="24">
+      <c r="K19" s="26">
+        <v>0.34266666666666701</v>
+      </c>
+      <c r="L19" s="25">
         <v>0.34866666666666701</v>
       </c>
-      <c r="L19" s="25">
+      <c r="M19" s="26">
         <v>0.19600000000000001</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="6" t="s">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B20" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="30">
+      <c r="C20" s="32">
         <v>3</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="27">
         <v>0.72799999999999998</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="26">
         <v>0.34399999999999997</v>
       </c>
-      <c r="G20" s="26">
+      <c r="G20" s="27">
         <v>0.224</v>
       </c>
-      <c r="H20" s="25">
+      <c r="H20" s="26">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I20" s="27">
+      <c r="I20" s="28">
         <v>21.3493654668837</v>
       </c>
-      <c r="J20" s="28">
+      <c r="J20" s="29">
         <v>1.74059399151431</v>
       </c>
-      <c r="K20" s="24">
+      <c r="K20" s="26">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="L20" s="25">
         <v>0.34066666666666701</v>
       </c>
-      <c r="L20" s="25">
+      <c r="M20" s="26">
         <v>0.19400000000000001</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B21" s="6" t="s">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B21" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="30">
+      <c r="C21" s="32">
         <v>9</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="27">
         <v>0.72733333333333305</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21" s="26">
         <v>0.34333333333333299</v>
       </c>
-      <c r="G21" s="26">
+      <c r="G21" s="27">
         <v>0.225333333333333</v>
       </c>
-      <c r="H21" s="25">
+      <c r="H21" s="26">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I21" s="27">
+      <c r="I21" s="28">
         <v>18.632597180447998</v>
       </c>
-      <c r="J21" s="28">
+      <c r="J21" s="29">
         <v>1.73229776052337</v>
       </c>
-      <c r="K21" s="24">
+      <c r="K21" s="26">
+        <v>0.214</v>
+      </c>
+      <c r="L21" s="25">
         <v>0.34</v>
       </c>
-      <c r="L21" s="25">
+      <c r="M21" s="26">
         <v>0.19400000000000001</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B22" s="6" t="s">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B22" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="30">
+      <c r="C22" s="32">
         <v>5</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="26">
+      <c r="E22" s="27">
         <v>0.69333333333333302</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="26">
         <v>0.27933333333333299</v>
       </c>
-      <c r="G22" s="26">
+      <c r="G22" s="27">
         <v>0.17066666666666699</v>
       </c>
-      <c r="H22" s="25">
+      <c r="H22" s="26">
         <v>0.23200000000000001</v>
       </c>
-      <c r="I22" s="27">
+      <c r="I22" s="28">
         <v>49.4875573431937</v>
       </c>
-      <c r="J22" s="28">
+      <c r="J22" s="29">
         <v>2.6932425632497301</v>
       </c>
-      <c r="K22" s="24">
+      <c r="K22" s="26">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="L22" s="25">
         <v>0.28266666666666701</v>
       </c>
-      <c r="L22" s="25">
+      <c r="M22" s="26">
         <v>0.139333333333333</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B23" s="6" t="s">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B23" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="30">
+      <c r="C23" s="32">
         <v>8</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="26">
+      <c r="E23" s="27">
         <v>0.68200000000000005</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F23" s="26">
         <v>0.27533333333333299</v>
       </c>
-      <c r="G23" s="26">
+      <c r="G23" s="27">
         <v>0.16866666666666699</v>
       </c>
-      <c r="H23" s="25">
+      <c r="H23" s="26">
         <v>0.22800000000000001</v>
       </c>
-      <c r="I23" s="27">
+      <c r="I23" s="28">
         <v>40.850487704099102</v>
       </c>
-      <c r="J23" s="28">
+      <c r="J23" s="29">
         <v>2.9670073640140902</v>
       </c>
-      <c r="K23" s="24">
+      <c r="K23" s="26">
+        <v>0.224</v>
+      </c>
+      <c r="L23" s="25">
         <v>0.27400000000000002</v>
       </c>
-      <c r="L23" s="25">
+      <c r="M23" s="26">
         <v>0.13866666666666699</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B24" s="6" t="s">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B24" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="30">
+      <c r="C24" s="32">
         <v>2</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="26">
+      <c r="E24" s="27">
         <v>0.68</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24" s="26">
         <v>0.274666666666667</v>
       </c>
-      <c r="G24" s="26">
+      <c r="G24" s="27">
         <v>0.16800000000000001</v>
       </c>
-      <c r="H24" s="25">
+      <c r="H24" s="26">
         <v>0.22900000000000001</v>
       </c>
-      <c r="I24" s="27">
+      <c r="I24" s="28">
         <v>41.166121356565299</v>
       </c>
-      <c r="J24" s="28">
+      <c r="J24" s="29">
         <v>3.0790369732270202</v>
       </c>
-      <c r="K24" s="24">
+      <c r="K24" s="26">
+        <v>0.276666666666667</v>
+      </c>
+      <c r="L24" s="25">
         <v>0.27200000000000002</v>
       </c>
-      <c r="L24" s="25">
+      <c r="M24" s="26">
         <v>0.13866666666666699</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B25" s="6" t="s">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B25" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="30">
+      <c r="C25" s="32">
         <v>4</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="26">
+      <c r="E25" s="27">
         <v>0.59733333333333305</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F25" s="26">
         <v>0.192</v>
       </c>
-      <c r="G25" s="26">
+      <c r="G25" s="27">
         <v>0.107333333333333</v>
       </c>
-      <c r="H25" s="25">
+      <c r="H25" s="26">
         <v>0.17399999999999999</v>
       </c>
-      <c r="I25" s="27">
+      <c r="I25" s="28">
         <v>60.482123266563399</v>
       </c>
-      <c r="J25" s="28">
+      <c r="J25" s="29">
         <v>4.4797837062111201</v>
       </c>
-      <c r="K25" s="24">
+      <c r="K25" s="26">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="L25" s="25">
         <v>0.19600000000000001</v>
       </c>
-      <c r="L25" s="25">
+      <c r="M25" s="26">
         <v>8.2666666666666694E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B26" s="6" t="s">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B26" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="30">
+      <c r="C26" s="32">
         <v>1</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="26">
+      <c r="E26" s="27">
         <v>0.56466666666666698</v>
       </c>
-      <c r="F26" s="25">
+      <c r="F26" s="26">
         <v>0.178666666666667</v>
       </c>
-      <c r="G26" s="26">
+      <c r="G26" s="27">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="H26" s="25">
+      <c r="H26" s="26">
         <v>0.16200000000000001</v>
       </c>
-      <c r="I26" s="27">
+      <c r="I26" s="28">
         <v>47.742502894621502</v>
       </c>
-      <c r="J26" s="28">
+      <c r="J26" s="29">
         <v>5.0634696284897096</v>
       </c>
-      <c r="K26" s="24">
+      <c r="K26" s="26">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="L26" s="25">
         <v>0.17533333333333301</v>
       </c>
-      <c r="L26" s="25">
+      <c r="M26" s="26">
         <v>7.9333333333333297E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B27" s="6" t="s">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B27" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="30">
+      <c r="C27" s="32">
         <v>7</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="26">
+      <c r="E27" s="27">
         <v>0.56399999999999995</v>
       </c>
-      <c r="F27" s="25">
+      <c r="F27" s="26">
         <v>0.17799999999999999</v>
       </c>
-      <c r="G27" s="26">
+      <c r="G27" s="27">
         <v>9.73333333333333E-2</v>
       </c>
-      <c r="H27" s="25">
+      <c r="H27" s="26">
         <v>0.16200000000000001</v>
       </c>
-      <c r="I27" s="27">
+      <c r="I27" s="28">
         <v>47.269390821496501</v>
       </c>
-      <c r="J27" s="28">
+      <c r="J27" s="29">
         <v>5.0593697058908003</v>
       </c>
-      <c r="K27" s="24">
+      <c r="K27" s="26">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="L27" s="25">
         <v>0.17733333333333301</v>
       </c>
-      <c r="L27" s="25">
+      <c r="M27" s="26">
         <v>7.9333333333333297E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C28" s="19"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="24"/>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="30"/>
       <c r="L28" s="25"/>
-    </row>
-    <row r="29" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="13" t="s">
+      <c r="M28" s="26"/>
+    </row>
+    <row r="29" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E29" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G29" s="14" t="s">
+      <c r="G29" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="H29" s="9" t="s">
+      <c r="H29" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I29" s="16" t="s">
+      <c r="I29" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="J29" s="15" t="s">
+      <c r="J29" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="K29" s="15" t="s">
+      <c r="K29" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="L29" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="L29" s="15" t="s">
+      <c r="M29" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="13" t="s">
+    <row r="30" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="15" t="s">
         <v>35</v>
       </c>
       <c r="H30" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="I30" s="16" t="s">
+      <c r="I30" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="J30" s="15" t="s">
+      <c r="J30" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="K30" s="15" t="s">
+      <c r="K30" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="L30" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="L30" s="15" t="s">
+      <c r="M30" s="16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B31" s="36" t="s">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B31" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C31" s="37">
+      <c r="C31" s="34">
         <v>10</v>
       </c>
-      <c r="D31" s="36" t="s">
+      <c r="D31" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="E31" s="26">
+      <c r="E31" s="27">
         <v>0.93600000000000005</v>
       </c>
-      <c r="F31" s="25">
+      <c r="F31" s="26">
         <v>0.580666666666667</v>
       </c>
-      <c r="G31" s="26">
+      <c r="G31" s="27">
         <v>0.40200000000000002</v>
       </c>
-      <c r="H31" s="25">
+      <c r="H31" s="26">
         <v>0.92100000000000004</v>
       </c>
-      <c r="I31" s="27">
-        <v>6.6670204160347701</v>
-      </c>
-      <c r="J31" s="28">
+      <c r="I31" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="J31" s="29">
         <v>0.13396314427199599</v>
       </c>
-      <c r="K31" s="24">
+      <c r="K31" s="26">
+        <v>1</v>
+      </c>
+      <c r="L31" s="25">
         <v>0.74133333333333296</v>
       </c>
-      <c r="L31" s="25">
+      <c r="M31" s="26">
         <v>0.72799999999999998</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B32" s="36" t="s">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B32" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="37">
+      <c r="C32" s="34">
         <v>6</v>
       </c>
-      <c r="D32" s="36" t="s">
+      <c r="D32" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="26">
+      <c r="E32" s="27">
         <v>0.91466666666666696</v>
       </c>
-      <c r="F32" s="25">
+      <c r="F32" s="26">
         <v>0.52733333333333299</v>
       </c>
-      <c r="G32" s="26">
+      <c r="G32" s="27">
         <v>0.36066666666666702</v>
       </c>
-      <c r="H32" s="25">
+      <c r="H32" s="26">
         <v>0.879</v>
       </c>
-      <c r="I32" s="27">
+      <c r="I32" s="28">
         <v>7.1191293053237699</v>
       </c>
-      <c r="J32" s="28">
+      <c r="J32" s="29">
         <v>1.97661140680339</v>
       </c>
-      <c r="K32" s="24">
+      <c r="K32" s="26">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="L32" s="25">
         <v>0.70266666666666699</v>
       </c>
-      <c r="L32" s="25">
+      <c r="M32" s="26">
         <v>0.67866666666666697</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B33" s="36" t="s">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B33" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="37">
+      <c r="C33" s="34">
         <v>3</v>
       </c>
-      <c r="D33" s="36" t="s">
+      <c r="D33" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="26">
+      <c r="E33" s="27">
         <v>0.913333333333333</v>
       </c>
-      <c r="F33" s="25">
+      <c r="F33" s="26">
         <v>0.52666666666666695</v>
       </c>
-      <c r="G33" s="26">
+      <c r="G33" s="27">
         <v>0.359333333333333</v>
       </c>
-      <c r="H33" s="25">
+      <c r="H33" s="26">
         <v>0.875</v>
       </c>
-      <c r="I33" s="27">
+      <c r="I33" s="28">
         <v>7.1177483321234796</v>
       </c>
-      <c r="J33" s="28">
+      <c r="J33" s="29">
         <v>1.9768417404393099</v>
       </c>
-      <c r="K33" s="24">
+      <c r="K33" s="26">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L33" s="25">
         <v>0.70066666666666699</v>
       </c>
-      <c r="L33" s="25">
+      <c r="M33" s="26">
         <v>0.67866666666666697</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B34" s="36" t="s">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B34" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="37">
+      <c r="C34" s="34">
         <v>9</v>
       </c>
-      <c r="D34" s="36" t="s">
+      <c r="D34" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="E34" s="26">
+      <c r="E34" s="27">
         <v>0.91266666666666696</v>
       </c>
-      <c r="F34" s="25">
+      <c r="F34" s="26">
         <v>0.52666666666666695</v>
       </c>
-      <c r="G34" s="26">
+      <c r="G34" s="27">
         <v>0.359333333333333</v>
       </c>
-      <c r="H34" s="25">
+      <c r="H34" s="26">
         <v>0.875</v>
       </c>
-      <c r="I34" s="27">
+      <c r="I34" s="28">
         <v>7.0995248993589399</v>
       </c>
-      <c r="J34" s="28">
+      <c r="J34" s="29">
         <v>1.98211338358807</v>
       </c>
-      <c r="K34" s="24">
+      <c r="K34" s="26">
+        <v>6.93333333333334E-2</v>
+      </c>
+      <c r="L34" s="25">
         <v>0.70066666666666699</v>
       </c>
-      <c r="L34" s="25">
+      <c r="M34" s="26">
         <v>0.67866666666666697</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B35" s="36" t="s">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B35" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C35" s="37">
+      <c r="C35" s="34">
         <v>5</v>
       </c>
-      <c r="D35" s="36" t="s">
+      <c r="D35" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="26">
+      <c r="E35" s="27">
         <v>0.86666666666666703</v>
       </c>
-      <c r="F35" s="25">
+      <c r="F35" s="26">
         <v>0.38400000000000001</v>
       </c>
-      <c r="G35" s="26">
+      <c r="G35" s="27">
         <v>0.24533333333333299</v>
       </c>
-      <c r="H35" s="25">
+      <c r="H35" s="26">
         <v>0.83199999999999996</v>
       </c>
-      <c r="I35" s="27">
+      <c r="I35" s="28">
         <v>29.470685373430399</v>
       </c>
-      <c r="J35" s="28">
+      <c r="J35" s="29">
         <v>7.6844016472097501</v>
       </c>
-      <c r="K35" s="24">
+      <c r="K35" s="26">
+        <v>8.9333333333333403E-2</v>
+      </c>
+      <c r="L35" s="25">
         <v>0.586666666666667</v>
       </c>
-      <c r="L35" s="25">
+      <c r="M35" s="26">
         <v>0.56599999999999995</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B36" s="36" t="s">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B36" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="37">
+      <c r="C36" s="34">
         <v>8</v>
       </c>
-      <c r="D36" s="36" t="s">
+      <c r="D36" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="26">
+      <c r="E36" s="27">
         <v>0.86466666666666703</v>
       </c>
-      <c r="F36" s="25">
+      <c r="F36" s="26">
         <v>0.38333333333333303</v>
       </c>
-      <c r="G36" s="26">
+      <c r="G36" s="27">
         <v>0.24333333333333301</v>
       </c>
-      <c r="H36" s="25">
+      <c r="H36" s="26">
         <v>0.82899999999999996</v>
       </c>
-      <c r="I36" s="27">
+      <c r="I36" s="28">
         <v>29.399475127366301</v>
       </c>
-      <c r="J36" s="28">
+      <c r="J36" s="29">
         <v>7.7067580284062096</v>
       </c>
-      <c r="K36" s="24">
+      <c r="K36" s="26">
+        <v>6.93333333333334E-2</v>
+      </c>
+      <c r="L36" s="25">
         <v>0.584666666666667</v>
       </c>
-      <c r="L36" s="25">
+      <c r="M36" s="26">
         <v>0.56533333333333302</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B37" s="36" t="s">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B37" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="37">
+      <c r="C37" s="34">
         <v>2</v>
       </c>
-      <c r="D37" s="36" t="s">
+      <c r="D37" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E37" s="26">
+      <c r="E37" s="27">
         <v>0.86466666666666703</v>
       </c>
-      <c r="F37" s="25">
+      <c r="F37" s="26">
         <v>0.38200000000000001</v>
       </c>
-      <c r="G37" s="26">
+      <c r="G37" s="27">
         <v>0.24399999999999999</v>
       </c>
-      <c r="H37" s="25">
+      <c r="H37" s="26">
         <v>0.82699999999999996</v>
       </c>
-      <c r="I37" s="27">
+      <c r="I37" s="28">
         <v>28.888510978104399</v>
       </c>
-      <c r="J37" s="28">
+      <c r="J37" s="29">
         <v>7.7314170901797796</v>
       </c>
-      <c r="K37" s="24">
+      <c r="K37" s="26">
+        <v>7.0666666666666697E-2</v>
+      </c>
+      <c r="L37" s="25">
         <v>0.58533333333333304</v>
       </c>
-      <c r="L37" s="25">
+      <c r="M37" s="26">
         <v>0.56333333333333302</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B38" s="36" t="s">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B38" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="37">
+      <c r="C38" s="34">
         <v>4</v>
       </c>
-      <c r="D38" s="36" t="s">
+      <c r="D38" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="26">
+      <c r="E38" s="27">
         <v>0.72666666666666702</v>
       </c>
-      <c r="F38" s="25">
+      <c r="F38" s="26">
         <v>0.231333333333333</v>
       </c>
-      <c r="G38" s="26">
+      <c r="G38" s="27">
         <v>0.133333333333333</v>
       </c>
-      <c r="H38" s="25">
+      <c r="H38" s="26">
         <v>0.69599999999999995</v>
       </c>
-      <c r="I38" s="27">
+      <c r="I38" s="28">
         <v>31.2975909466467</v>
       </c>
-      <c r="J38" s="28">
+      <c r="J38" s="29">
         <v>13.087751395539501</v>
       </c>
-      <c r="K38" s="24">
+      <c r="K38" s="26">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="L38" s="25">
         <v>0.41</v>
       </c>
-      <c r="L38" s="25">
+      <c r="M38" s="26">
         <v>0.38800000000000001</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B39" s="36" t="s">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B39" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C39" s="37">
+      <c r="C39" s="34">
         <v>7</v>
       </c>
-      <c r="D39" s="36" t="s">
+      <c r="D39" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E39" s="26">
+      <c r="E39" s="27">
         <v>0.72</v>
       </c>
-      <c r="F39" s="25">
+      <c r="F39" s="26">
         <v>0.22666666666666699</v>
       </c>
-      <c r="G39" s="26">
+      <c r="G39" s="27">
         <v>0.13200000000000001</v>
       </c>
-      <c r="H39" s="25">
+      <c r="H39" s="26">
         <v>0.68700000000000006</v>
       </c>
-      <c r="I39" s="27">
+      <c r="I39" s="28">
         <v>30.704325579053101</v>
       </c>
-      <c r="J39" s="28">
+      <c r="J39" s="29">
         <v>13.2330532798274</v>
       </c>
-      <c r="K39" s="24">
+      <c r="K39" s="26">
+        <v>7.0666666666666697E-2</v>
+      </c>
+      <c r="L39" s="25">
         <v>0.40266666666666701</v>
       </c>
-      <c r="L39" s="25">
+      <c r="M39" s="26">
         <v>0.38133333333333302</v>
       </c>
     </row>
-    <row r="40" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="38" t="s">
+    <row r="40" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="39">
+      <c r="C40" s="36">
         <v>1</v>
       </c>
-      <c r="D40" s="38" t="s">
+      <c r="D40" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E40" s="31">
+      <c r="E40" s="37">
         <v>0.71866666666666701</v>
       </c>
-      <c r="F40" s="32">
+      <c r="F40" s="38">
         <v>0.22666666666666699</v>
       </c>
-      <c r="G40" s="31">
+      <c r="G40" s="37">
         <v>0.131333333333333</v>
       </c>
-      <c r="H40" s="32">
+      <c r="H40" s="38">
         <v>0.68700000000000006</v>
       </c>
-      <c r="I40" s="33">
+      <c r="I40" s="39">
         <v>30.464933518121601</v>
       </c>
-      <c r="J40" s="34">
+      <c r="J40" s="40">
         <v>13.299213010558001</v>
       </c>
-      <c r="K40" s="35">
+      <c r="K40" s="38">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="L40" s="41">
         <v>0.40133333333333299</v>
       </c>
-      <c r="L40" s="32">
+      <c r="M40" s="38">
         <v>0.38</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B31:L40">
+  <sortState ref="B31:M40">
     <sortCondition descending="1" ref="E31:E40"/>
     <sortCondition descending="1" ref="F31:F40"/>
     <sortCondition ref="I31:I40"/>
-    <sortCondition descending="1" ref="J31:J40"/>
+    <sortCondition descending="1" ref="K31:K40"/>
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>